<commit_message>
sql exercice en cours
</commit_message>
<xml_diff>
--- a/03-Databases/cours/03 - Databases/matrice-Bibliothèque.xlsx
+++ b/03-Databases/cours/03 - Databases/matrice-Bibliothèque.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdevoldere\Documents\GitHub\DWWM_2409\03 - Databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bherault\Documents\GitHub\DWWM_2409_HB\03-Databases\cours\03 - Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493277B0-4131-45EA-AD9D-2C2E714E974B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD2036F-8F7B-4CEA-8A5A-EBD2AFE357E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>client_id</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avec un client id je peux trouver un client nom prenom adres caution </t>
   </si>
 </sst>
 </file>
@@ -175,10 +178,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3FFBC9BA-9027-4E46-A078-4235C90E9092}" name="Tableau3" displayName="Tableau3" ref="B3:E16" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3FFBC9BA-9027-4E46-A078-4235C90E9092}" name="Tableau3" displayName="Tableau3" ref="B3:E16" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="B3:E16" xr:uid="{3FFBC9BA-9027-4E46-A078-4235C90E9092}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9AB9149E-1AE9-4EB8-8CB5-AC017EAF36FD}" name="\" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{9AB9149E-1AE9-4EB8-8CB5-AC017EAF36FD}" name="\" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{032BA5AB-4852-4F3E-AFB6-BD84CF3F62CC}" name="client_id"/>
     <tableColumn id="6" xr3:uid="{19602AE2-AA02-4D16-B619-2FB56C809994}" name="book_id"/>
     <tableColumn id="11" xr3:uid="{5268B891-EFA9-4C31-85BC-CE553AD9A00B}" name="author_id"/>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E16"/>
+  <dimension ref="B3:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,9 +465,10 @@
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="7" max="7" width="66.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
@@ -477,13 +481,16 @@
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -491,7 +498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -499,7 +506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -507,12 +514,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -520,7 +527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -528,7 +535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -536,7 +543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -544,12 +551,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -557,12 +564,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>